<commit_message>
improve oil pressure reading?
</commit_message>
<xml_diff>
--- a/references/oil pressure.xlsx
+++ b/references/oil pressure.xlsx
@@ -8,17 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.bousquet\Documents\code\perso\bb_dash\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC7A4A2-251A-4865-9B22-20616E89DF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0C4DDC-644E-4019-A05B-D672F54C6A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5EDB769B-7CD3-4D9A-B2D6-6220D20AC783}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EDB769B-7CD3-4D9A-B2D6-6220D20AC783}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$B$2:$F$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$B$3:$F$3</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -68,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -109,8 +105,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1182,6 +1178,130 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$F$19:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>95.972090072946401</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.599429115128444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$G$19:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A91C-4F00-A6B1-1E1885560F2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$F$19:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>95.972090072946401</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.599429115128444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$H$19:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A91C-4F00-A6B1-1E1885560F2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2855,15 +2975,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743D8DBB-F68F-4B65-A4A5-F1BD2E61CF2C}">
-  <dimension ref="A2:H21"/>
+  <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2883,7 +3003,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2903,7 +3023,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2923,7 +3043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2941,28 +3061,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>120</v>
       </c>
       <c r="B7" s="3">
-        <f>(1/(1/B$3+1/$A7))*(B$4/(1/(1/B$3+1/$A7)+B$2))/30*1024</f>
+        <f t="shared" ref="B7:F10" si="0">(1/(1/B$3+1/$A7))*(B$4/(1/(1/B$3+1/$A7)+B$2))/30*1024</f>
         <v>156.99156925256818</v>
       </c>
       <c r="C7" s="3">
-        <f>(1/(1/C$3+1/$A7))*(C$4/(1/(1/C$3+1/$A7)+C$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>156.9979232505643</v>
       </c>
       <c r="D7" s="3">
-        <f>(1/(1/D$3+1/$A7))*(D$4/(1/(1/D$3+1/$A7)+D$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>157.00963724959396</v>
       </c>
       <c r="E7" s="3">
-        <f>(1/(1/E$3+1/$A7))*(E$4/(1/(1/E$3+1/$A7)+E$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>157.02347696879642</v>
       </c>
       <c r="F7" s="3">
-        <f>(1/(1/F$3+1/$A7))*(F$4/(1/(1/F$3+1/$A7)+F$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>157.03672646643824</v>
       </c>
       <c r="G7">
@@ -2973,28 +3093,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>52</v>
       </c>
       <c r="B8" s="3">
-        <f>(1/(1/B$3+1/$A8))*(B$4/(1/(1/B$3+1/$A8)+B$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>125.5323688338853</v>
       </c>
       <c r="C8" s="3">
-        <f>(1/(1/C$3+1/$A8))*(C$4/(1/(1/C$3+1/$A8)+C$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>117.6759038967124</v>
       </c>
       <c r="D8" s="3">
-        <f>(1/(1/D$3+1/$A8))*(D$4/(1/(1/D$3+1/$A8)+D$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>115.86859065972062</v>
       </c>
       <c r="E8" s="3">
-        <f>(1/(1/E$3+1/$A8))*(E$4/(1/(1/E$3+1/$A8)+E$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>110.75446630119315</v>
       </c>
       <c r="F8" s="3">
-        <f>(1/(1/F$3+1/$A8))*(F$4/(1/(1/F$3+1/$A8)+F$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>99.082038037097888</v>
       </c>
       <c r="G8">
@@ -3005,28 +3125,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>41</v>
       </c>
       <c r="B9" s="3">
-        <f>(1/(1/B$3+1/$A9))*(B$4/(1/(1/B$3+1/$A9)+B$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>114.6545046125112</v>
       </c>
       <c r="C9" s="3">
-        <f>(1/(1/C$3+1/$A9))*(C$4/(1/(1/C$3+1/$A9)+C$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>105.20085295398033</v>
       </c>
       <c r="D9" s="3">
-        <f>(1/(1/D$3+1/$A9))*(D$4/(1/(1/D$3+1/$A9)+D$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>103.08047388064554</v>
       </c>
       <c r="E9" s="3">
-        <f>(1/(1/E$3+1/$A9))*(E$4/(1/(1/E$3+1/$A9)+E$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>97.194777693032421</v>
       </c>
       <c r="F9" s="3">
-        <f>(1/(1/F$3+1/$A9))*(F$4/(1/(1/F$3+1/$A9)+F$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>84.344490390861424</v>
       </c>
       <c r="G9">
@@ -3037,39 +3157,39 @@
         <v>2109.21</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" s="3">
-        <f>(1/(1/B$3+1/$A10))*(B$4/(1/(1/B$3+1/$A10)+B$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>69.908857165391581</v>
       </c>
       <c r="C10" s="3">
-        <f>(1/(1/C$3+1/$A10))*(C$4/(1/(1/C$3+1/$A10)+C$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>59.000746521886661</v>
       </c>
       <c r="D10" s="3">
-        <f>(1/(1/D$3+1/$A10))*(D$4/(1/(1/D$3+1/$A10)+D$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>56.786958437362308</v>
       </c>
       <c r="E10" s="3">
-        <f>(1/(1/E$3+1/$A10))*(E$4/(1/(1/E$3+1/$A10)+E$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>51.039265877807303</v>
       </c>
       <c r="F10" s="3">
-        <f>(1/(1/F$3+1/$A10))*(F$4/(1/(1/F$3+1/$A10)+F$2))/30*1024</f>
+        <f t="shared" si="0"/>
         <v>40.189801129768632</v>
       </c>
       <c r="G10">
         <v>90</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" ref="H9:H10" si="0">G10*70.307</f>
+        <f t="shared" ref="H10" si="1">G10*70.307</f>
         <v>6327.63</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>-2.5499999999999998E-2</v>
       </c>
@@ -3086,7 +3206,7 @@
         <v>-1.15E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>3.3607</v>
       </c>
@@ -3103,7 +3223,7 @@
         <v>7.22E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3750</v>
       </c>
@@ -3123,7 +3243,7 @@
         <v>105.66</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f>A15/30000*1024</f>
         <v>128</v>
@@ -3133,45 +3253,45 @@
         <v>-8.068399999999972</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:F16" si="1">C13*$A$16*$A$16+C14*$A$16+C15</f>
+        <f t="shared" ref="C16:F16" si="2">C13*$A$16*$A$16+C14*$A$16+C15</f>
         <v>-29.243869999999973</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-33.840240000000009</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-46.261880000000005</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-73.514399999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>B16*70.307</f>
         <v>-567.26499879999801</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:F17" si="2">C16*70.307</f>
+        <f t="shared" ref="C17:F17" si="3">C16*70.307</f>
         <v>-2056.0487680899982</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2379.2057536800007</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3252.5339971600006</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5168.5769208000002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3750</v>
       </c>
@@ -3182,29 +3302,61 @@
       <c r="C19">
         <v>500</v>
       </c>
+      <c r="F19">
+        <f>(G19-10565)/-78.825</f>
+        <v>95.972090072946401</v>
+      </c>
+      <c r="G19">
+        <v>3000</v>
+      </c>
+      <c r="H19">
+        <v>2200</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2636</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20:B21" si="3">A20/30000*1024</f>
+        <f t="shared" ref="B20:B21" si="4">A20/30000*1024</f>
         <v>89.975466666666662</v>
       </c>
       <c r="C20">
         <v>3500</v>
       </c>
+      <c r="F20">
+        <f>(G20-10565)/-78.825</f>
+        <v>70.599429115128444</v>
+      </c>
+      <c r="G20">
+        <v>5000</v>
+      </c>
+      <c r="H20">
+        <v>4000</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3164</v>
       </c>
       <c r="B21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>107.99786666666667</v>
       </c>
       <c r="C21">
         <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <f>SLOPE(H19:H20,F19:F20)</f>
+        <v>-70.942499999999981</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f>INTERCEPT(H19:H20,F19:F20)</f>
+        <v>9008.4999999999982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>